<commit_message>
working framework with multiple ArrayList methods, csv output and parameters allowing multiple tests at a time
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tinygobby/Desktop/Projects/Makers/Week_10/algorithmic-complexity/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133718FA-9FD8-C446-A57D-5936CC6B190C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439E7061-8822-C844-81DF-0BBA7F9396CB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{55AD68BF-37E3-EA42-BDC5-DFDA6E8E6F44}"/>
+    <workbookView xWindow="21780" yWindow="-21140" windowWidth="19200" windowHeight="21140" activeTab="2" xr2:uid="{55AD68BF-37E3-EA42-BDC5-DFDA6E8E6F44}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Reverse</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Sort</t>
+  </si>
+  <si>
+    <t>Shuffle(μs)</t>
+  </si>
+  <si>
+    <t>Sort(μs)</t>
+  </si>
+  <si>
+    <t>1000 iterations</t>
   </si>
 </sst>
 </file>
@@ -184,7 +193,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Overall!$A$2</c:f>
+              <c:f>Overall!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -205,41 +214,80 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
               <c:f>Overall!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.89400000000000002</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82699999999999996</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78200000000000003</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78500000000000003</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79500000000000004</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.83699999999999997</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.80100000000000005</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.82</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81799999999999995</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.81299999999999994</c:v>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>894</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>827</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>782</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>837</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>818</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>813</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -256,7 +304,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Overall!$B$2</c:f>
+              <c:f>Overall!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -277,9 +325,48 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Overall!$A$3:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Overall!$B$3:$B$12</c:f>
+              <c:f>Overall!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -328,7 +415,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Overall!$C$2</c:f>
+              <c:f>Overall!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -349,41 +436,80 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Overall!$C$3:$C$12</c:f>
+              <c:f>Overall!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1294.5999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2832.7000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3793.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5745.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6641.4000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8239.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9107.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11784.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13090.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13817.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,7 +526,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Overall!$D$2</c:f>
+              <c:f>Overall!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -421,41 +547,80 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>Overall!$D$3:$D$12</c:f>
+              <c:f>Overall!$A$3:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>8000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>9000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>219.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>482.30000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>704.19999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>858.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>993.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1160.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1599.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1853.6000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2100.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,44 +649,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="220583199"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -534,7 +667,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -554,33 +687,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="220564479"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1366,6 +1472,36 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>12.946</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.327000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.935000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.454000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>66.414000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.393000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91.073999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>117.846</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130.90899999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>138.179</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1636,6 +1772,36 @@
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.1930000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8230000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0419999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5860000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9320000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.605</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.994999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.536000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.001000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4594,13 +4760,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -5098,211 +5264,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909E9FA2-7A70-DD4C-B25A-29F9079A6979}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>Last!C3</f>
-        <v>0.89400000000000002</v>
+        <v>1000</v>
       </c>
       <c r="B3">
+        <f>Last!C3 * 1000</f>
+        <v>894</v>
+      </c>
+      <c r="C3">
         <f>Reverse!C3</f>
         <v>585.88300000000004</v>
       </c>
-      <c r="C3">
-        <f>Shuffle!C3</f>
-        <v>0</v>
-      </c>
       <c r="D3">
-        <f>Sort!C3</f>
-        <v>0</v>
+        <f>Shuffle!C3 * 100</f>
+        <v>1294.5999999999999</v>
+      </c>
+      <c r="E3">
+        <f>Sort!C3*100</f>
+        <v>219.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f>Last!C4</f>
-        <v>0.82699999999999996</v>
+        <v>2000</v>
       </c>
       <c r="B4">
+        <f>Last!C4 * 1000</f>
+        <v>827</v>
+      </c>
+      <c r="C4">
         <f>Reverse!C4</f>
         <v>1099.874</v>
       </c>
-      <c r="C4">
-        <f>Shuffle!C4</f>
-        <v>0</v>
-      </c>
       <c r="D4">
-        <f>Sort!C4</f>
-        <v>0</v>
+        <f>Shuffle!C4 * 100</f>
+        <v>2832.7000000000003</v>
+      </c>
+      <c r="E4">
+        <f>Sort!C4*100</f>
+        <v>482.30000000000007</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f>Last!C5</f>
-        <v>0.78200000000000003</v>
+        <v>3000</v>
       </c>
       <c r="B5">
+        <f>Last!C5 * 1000</f>
+        <v>782</v>
+      </c>
+      <c r="C5">
         <f>Reverse!C5</f>
         <v>1764.2070000000001</v>
       </c>
-      <c r="C5">
-        <f>Shuffle!C5</f>
-        <v>0</v>
-      </c>
       <c r="D5">
-        <f>Sort!C5</f>
-        <v>0</v>
+        <f>Shuffle!C5 * 100</f>
+        <v>3793.5</v>
+      </c>
+      <c r="E5">
+        <f>Sort!C5*100</f>
+        <v>704.19999999999993</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <f>Last!C6</f>
-        <v>0.78500000000000003</v>
+        <v>4000</v>
       </c>
       <c r="B6">
+        <f>Last!C6 * 1000</f>
+        <v>785</v>
+      </c>
+      <c r="C6">
         <f>Reverse!C6</f>
         <v>2315.3490000000002</v>
       </c>
-      <c r="C6">
-        <f>Shuffle!C6</f>
-        <v>0</v>
-      </c>
       <c r="D6">
-        <f>Sort!C6</f>
-        <v>0</v>
+        <f>Shuffle!C6 * 100</f>
+        <v>5745.4</v>
+      </c>
+      <c r="E6">
+        <f>Sort!C6*100</f>
+        <v>858.6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <f>Last!C7</f>
-        <v>0.79500000000000004</v>
+        <v>5000</v>
       </c>
       <c r="B7">
+        <f>Last!C7 * 1000</f>
+        <v>795</v>
+      </c>
+      <c r="C7">
         <f>Reverse!C7</f>
         <v>2850.9769999999999</v>
       </c>
-      <c r="C7">
-        <f>Shuffle!C7</f>
-        <v>0</v>
-      </c>
       <c r="D7">
-        <f>Sort!C7</f>
-        <v>0</v>
+        <f>Shuffle!C7 * 100</f>
+        <v>6641.4000000000005</v>
+      </c>
+      <c r="E7">
+        <f>Sort!C7*100</f>
+        <v>993.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <f>Last!C8</f>
-        <v>0.83699999999999997</v>
+        <v>6000</v>
       </c>
       <c r="B8">
+        <f>Last!C8 * 1000</f>
+        <v>837</v>
+      </c>
+      <c r="C8">
         <f>Reverse!C8</f>
         <v>3697.7260000000001</v>
       </c>
-      <c r="C8">
-        <f>Shuffle!C8</f>
-        <v>0</v>
-      </c>
       <c r="D8">
-        <f>Sort!C8</f>
-        <v>0</v>
+        <f>Shuffle!C8 * 100</f>
+        <v>8239.2999999999993</v>
+      </c>
+      <c r="E8">
+        <f>Sort!C8*100</f>
+        <v>1160.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <f>Last!C9</f>
-        <v>0.80100000000000005</v>
+        <v>7000</v>
       </c>
       <c r="B9">
+        <f>Last!C9 * 1000</f>
+        <v>801</v>
+      </c>
+      <c r="C9">
         <f>Reverse!C9</f>
         <v>3882.3739999999998</v>
       </c>
-      <c r="C9">
-        <f>Shuffle!C9</f>
-        <v>0</v>
-      </c>
       <c r="D9">
-        <f>Sort!C9</f>
-        <v>0</v>
+        <f>Shuffle!C9 * 100</f>
+        <v>9107.4</v>
+      </c>
+      <c r="E9">
+        <f>Sort!C9*100</f>
+        <v>1599.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <f>Last!C10</f>
-        <v>0.82</v>
+        <v>8000</v>
       </c>
       <c r="B10">
+        <f>Last!C10 * 1000</f>
+        <v>820</v>
+      </c>
+      <c r="C10">
         <f>Reverse!C10</f>
         <v>4622.317</v>
       </c>
-      <c r="C10">
-        <f>Shuffle!C10</f>
-        <v>0</v>
-      </c>
       <c r="D10">
-        <f>Sort!C10</f>
-        <v>0</v>
+        <f>Shuffle!C10 * 100</f>
+        <v>11784.6</v>
+      </c>
+      <c r="E10">
+        <f>Sort!C10*100</f>
+        <v>1853.6000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <f>Last!C11</f>
-        <v>0.81799999999999995</v>
+        <v>9000</v>
       </c>
       <c r="B11">
+        <f>Last!C11 * 1000</f>
+        <v>818</v>
+      </c>
+      <c r="C11">
         <f>Reverse!C11</f>
         <v>5279.2849999999999</v>
       </c>
-      <c r="C11">
-        <f>Shuffle!C11</f>
-        <v>0</v>
-      </c>
       <c r="D11">
-        <f>Sort!C11</f>
-        <v>0</v>
+        <f>Shuffle!C11 * 100</f>
+        <v>13090.9</v>
+      </c>
+      <c r="E11">
+        <f>Sort!C11*100</f>
+        <v>2018</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <f>Last!C12</f>
-        <v>0.81299999999999994</v>
+        <v>10000</v>
       </c>
       <c r="B12">
+        <f>Last!C12 * 1000</f>
+        <v>813</v>
+      </c>
+      <c r="C12">
         <f>Reverse!C12</f>
         <v>5834.9219999999996</v>
       </c>
-      <c r="C12">
-        <f>Shuffle!C12</f>
-        <v>0</v>
-      </c>
       <c r="D12">
-        <f>Sort!C12</f>
-        <v>0</v>
+        <f>Shuffle!C12 * 100</f>
+        <v>13817.9</v>
+      </c>
+      <c r="E12">
+        <f>Sort!C12*100</f>
+        <v>2100.1</v>
       </c>
     </row>
   </sheetData>
@@ -5535,8 +5731,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5755,7 +5951,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5766,7 +5962,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -5796,91 +5992,171 @@
       <c r="A3">
         <v>1000</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="B3" s="1">
+        <v>11.263999999999999</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12.946</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19.21</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.3049999999999999</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2000</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B4" s="1">
+        <v>24.885000000000002</v>
+      </c>
+      <c r="C4" s="1">
+        <v>28.327000000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <v>32.228000000000002</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.7170000000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3000</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="1">
+        <v>34.744999999999997</v>
+      </c>
+      <c r="C5" s="1">
+        <v>37.935000000000002</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41.807000000000002</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.266</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4000</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6" s="1">
+        <v>53.042999999999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>57.454000000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>64.114999999999995</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.173</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5000</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="1">
+        <v>60.988999999999997</v>
+      </c>
+      <c r="C7" s="1">
+        <v>66.414000000000001</v>
+      </c>
+      <c r="D7" s="1">
+        <v>74.418000000000006</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.65</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6000</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="1">
+        <v>74.878</v>
+      </c>
+      <c r="C8" s="1">
+        <v>82.393000000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>93.391000000000005</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3.722</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7000</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="1">
+        <v>83.186000000000007</v>
+      </c>
+      <c r="C9" s="1">
+        <v>91.073999999999998</v>
+      </c>
+      <c r="D9" s="1">
+        <v>108.758</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5.0650000000000004</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8000</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="1">
+        <v>97.543999999999997</v>
+      </c>
+      <c r="C10" s="1">
+        <v>117.846</v>
+      </c>
+      <c r="D10" s="1">
+        <v>146.65</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.31</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9000</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="1">
+        <v>118.986</v>
+      </c>
+      <c r="C11" s="1">
+        <v>130.90899999999999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>155.76</v>
+      </c>
+      <c r="E11" s="1">
+        <v>7.3959999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10000</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="B12" s="1">
+        <v>112.122</v>
+      </c>
+      <c r="C12" s="1">
+        <v>138.179</v>
+      </c>
+      <c r="D12" s="1">
+        <v>174.333</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.3480000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5894,7 +6170,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5905,13 +6181,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -5935,91 +6211,171 @@
       <c r="A3">
         <v>1000</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="B3" s="1">
+        <v>1.732</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.1930000000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.3659999999999997</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.37</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2000</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="B4" s="1">
+        <v>3.863</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.8230000000000004</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.8420000000000005</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.097</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3000</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="1">
+        <v>6.07</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.0419999999999998</v>
+      </c>
+      <c r="D5" s="1">
+        <v>12.241</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.85399999999999998</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4000</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6" s="1">
+        <v>6.3710000000000004</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.5860000000000003</v>
+      </c>
+      <c r="D6" s="1">
+        <v>29.074000000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.383</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5000</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="1">
+        <v>8.5229999999999997</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.9320000000000004</v>
+      </c>
+      <c r="D7" s="1">
+        <v>15.78</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.89200000000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6000</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="1">
+        <v>10.371</v>
+      </c>
+      <c r="C8" s="1">
+        <v>11.605</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20.387</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.1180000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7000</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="1">
+        <v>11.013999999999999</v>
+      </c>
+      <c r="C9" s="1">
+        <v>15.994999999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>25.608000000000001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.6379999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8000</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="1">
+        <v>14.975</v>
+      </c>
+      <c r="C10" s="1">
+        <v>18.536000000000001</v>
+      </c>
+      <c r="D10" s="1">
+        <v>40.222000000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3.4060000000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9000</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="1">
+        <v>15.438000000000001</v>
+      </c>
+      <c r="C11" s="1">
+        <v>20.18</v>
+      </c>
+      <c r="D11" s="1">
+        <v>27.602</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.0529999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10000</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="B12" s="1">
+        <v>17.486000000000001</v>
+      </c>
+      <c r="C12" s="1">
+        <v>21.001000000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>30.957999999999998</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.0019999999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>